<commit_message>
update summary and template
</commit_message>
<xml_diff>
--- a/public/assets/file/idp_template.xlsx
+++ b/public/assets/file/idp_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itd.magang02\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77A7445-FB2B-497F-BF52-C3E15DDFF2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B183C583-4CBD-468D-97C3-24540E4CCCB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,7 +189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,6 +402,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="28"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1107,7 +1122,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="231">
+  <cellXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1165,9 +1180,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
@@ -1233,6 +1245,375 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="54" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="54" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1245,12 +1626,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1263,497 +1638,134 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="54" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="29" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="29" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="30" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="29" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="45" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="29" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3467,8 +3479,8 @@
   </sheetPr>
   <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33:W33"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="43.15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4940,836 +4952,836 @@
       <c r="X2" s="120"/>
     </row>
     <row r="3" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="44" t="s">
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43" t="s">
+      <c r="F3" s="42"/>
+      <c r="G3" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="44" t="s">
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43" t="s">
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="157"/>
-      <c r="S3" s="157"/>
-      <c r="T3" s="158"/>
-      <c r="U3" s="91"/>
-      <c r="V3" s="92"/>
-      <c r="W3" s="92"/>
-      <c r="X3" s="92"/>
+      <c r="R3" s="110"/>
+      <c r="S3" s="110"/>
+      <c r="T3" s="111"/>
+      <c r="U3" s="121"/>
+      <c r="V3" s="122"/>
+      <c r="W3" s="122"/>
+      <c r="X3" s="122"/>
     </row>
     <row r="4" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="38" t="s">
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37" t="s">
+      <c r="F4" s="36"/>
+      <c r="G4" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="121" t="s">
+      <c r="H4" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="121"/>
-      <c r="J4" s="121"/>
-      <c r="K4" s="122"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="38" t="s">
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="113"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37" t="s">
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="R4" s="155"/>
-      <c r="S4" s="155"/>
-      <c r="T4" s="156"/>
-      <c r="U4" s="91"/>
-      <c r="V4" s="92"/>
-      <c r="W4" s="92"/>
-      <c r="X4" s="92"/>
+      <c r="R4" s="108"/>
+      <c r="S4" s="108"/>
+      <c r="T4" s="109"/>
+      <c r="U4" s="121"/>
+      <c r="V4" s="122"/>
+      <c r="W4" s="122"/>
+      <c r="X4" s="122"/>
     </row>
     <row r="5" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="38" t="s">
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37" t="s">
+      <c r="F5" s="36"/>
+      <c r="G5" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="41" t="s">
+      <c r="H5" s="41"/>
+      <c r="I5" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="39" t="s">
+      <c r="J5" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="40"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="38" t="s">
+      <c r="K5" s="39"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37" t="s">
+      <c r="P5" s="36"/>
+      <c r="Q5" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="153"/>
-      <c r="S5" s="153"/>
-      <c r="T5" s="154"/>
-      <c r="U5" s="91"/>
-      <c r="V5" s="92"/>
-      <c r="W5" s="92"/>
-      <c r="X5" s="92"/>
+      <c r="R5" s="151"/>
+      <c r="S5" s="151"/>
+      <c r="T5" s="152"/>
+      <c r="U5" s="121"/>
+      <c r="V5" s="122"/>
+      <c r="W5" s="122"/>
+      <c r="X5" s="122"/>
     </row>
     <row r="6" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="38" t="s">
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37" t="s">
+      <c r="F6" s="36"/>
+      <c r="G6" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="121"/>
-      <c r="J6" s="121"/>
-      <c r="K6" s="122"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="38" t="s">
+      <c r="H6" s="38"/>
+      <c r="I6" s="112"/>
+      <c r="J6" s="112"/>
+      <c r="K6" s="113"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37" t="s">
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="R6" s="98"/>
-      <c r="S6" s="98"/>
-      <c r="T6" s="99"/>
-      <c r="U6" s="91"/>
-      <c r="V6" s="92"/>
-      <c r="W6" s="92"/>
-      <c r="X6" s="92"/>
+      <c r="R6" s="160"/>
+      <c r="S6" s="160"/>
+      <c r="T6" s="161"/>
+      <c r="U6" s="121"/>
+      <c r="V6" s="122"/>
+      <c r="W6" s="122"/>
+      <c r="X6" s="122"/>
     </row>
     <row r="7" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="O7" s="94" t="s">
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="O7" s="156" t="s">
         <v>19</v>
       </c>
-      <c r="P7" s="95"/>
-      <c r="Q7" s="56" t="s">
+      <c r="P7" s="157"/>
+      <c r="Q7" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="R7" s="96"/>
-      <c r="S7" s="96"/>
-      <c r="T7" s="97"/>
-      <c r="U7" s="93"/>
-      <c r="V7" s="61"/>
-      <c r="W7" s="61"/>
-      <c r="X7" s="61"/>
+      <c r="R7" s="158"/>
+      <c r="S7" s="158"/>
+      <c r="T7" s="159"/>
+      <c r="U7" s="169"/>
+      <c r="V7" s="62"/>
+      <c r="W7" s="62"/>
+      <c r="X7" s="62"/>
     </row>
     <row r="8" spans="1:24" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="100"/>
-      <c r="P8" s="100"/>
-      <c r="Q8" s="100"/>
-      <c r="R8" s="100"/>
-      <c r="S8" s="100"/>
-      <c r="T8" s="100"/>
-      <c r="U8" s="100"/>
-      <c r="V8" s="100"/>
-      <c r="W8" s="100"/>
-      <c r="X8" s="100"/>
+      <c r="B8" s="170"/>
+      <c r="C8" s="170"/>
+      <c r="D8" s="170"/>
+      <c r="E8" s="170"/>
+      <c r="F8" s="170"/>
+      <c r="G8" s="170"/>
+      <c r="H8" s="170"/>
+      <c r="I8" s="170"/>
+      <c r="J8" s="170"/>
+      <c r="K8" s="170"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="162"/>
+      <c r="P8" s="162"/>
+      <c r="Q8" s="162"/>
+      <c r="R8" s="162"/>
+      <c r="S8" s="162"/>
+      <c r="T8" s="162"/>
+      <c r="U8" s="162"/>
+      <c r="V8" s="162"/>
+      <c r="W8" s="162"/>
+      <c r="X8" s="162"/>
     </row>
     <row r="9" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
-      <c r="B9" s="126" t="s">
+      <c r="A9" s="34"/>
+      <c r="B9" s="124" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="126"/>
-      <c r="D9" s="126"/>
-      <c r="E9" s="126"/>
-      <c r="F9" s="126"/>
-      <c r="G9" s="126"/>
-      <c r="H9" s="126"/>
-      <c r="I9" s="126"/>
-      <c r="J9" s="126"/>
-      <c r="K9" s="126"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="128" t="s">
+      <c r="C9" s="124"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="124"/>
+      <c r="F9" s="124"/>
+      <c r="G9" s="124"/>
+      <c r="H9" s="124"/>
+      <c r="I9" s="124"/>
+      <c r="J9" s="124"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="P9" s="129"/>
-      <c r="Q9" s="129"/>
-      <c r="R9" s="129"/>
-      <c r="S9" s="129"/>
-      <c r="T9" s="129"/>
-      <c r="U9" s="129"/>
-      <c r="V9" s="129"/>
-      <c r="W9" s="130"/>
+      <c r="P9" s="127"/>
+      <c r="Q9" s="127"/>
+      <c r="R9" s="127"/>
+      <c r="S9" s="127"/>
+      <c r="T9" s="127"/>
+      <c r="U9" s="127"/>
+      <c r="V9" s="127"/>
+      <c r="W9" s="128"/>
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="127"/>
-      <c r="C10" s="127"/>
-      <c r="D10" s="127"/>
-      <c r="E10" s="127"/>
-      <c r="F10" s="127"/>
-      <c r="G10" s="127"/>
-      <c r="H10" s="127"/>
-      <c r="I10" s="127"/>
-      <c r="J10" s="127"/>
-      <c r="K10" s="127"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="131"/>
-      <c r="P10" s="131"/>
-      <c r="Q10" s="131"/>
-      <c r="R10" s="131"/>
-      <c r="S10" s="131"/>
-      <c r="T10" s="131"/>
-      <c r="U10" s="131"/>
-      <c r="V10" s="131"/>
-      <c r="W10" s="132"/>
+      <c r="B10" s="125"/>
+      <c r="C10" s="125"/>
+      <c r="D10" s="125"/>
+      <c r="E10" s="125"/>
+      <c r="F10" s="125"/>
+      <c r="G10" s="125"/>
+      <c r="H10" s="125"/>
+      <c r="I10" s="125"/>
+      <c r="J10" s="125"/>
+      <c r="K10" s="125"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="129"/>
+      <c r="P10" s="129"/>
+      <c r="Q10" s="129"/>
+      <c r="R10" s="129"/>
+      <c r="S10" s="129"/>
+      <c r="T10" s="129"/>
+      <c r="U10" s="129"/>
+      <c r="V10" s="129"/>
+      <c r="W10" s="130"/>
       <c r="X10" s="3"/>
     </row>
     <row r="11" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="133" t="s">
+      <c r="B11" s="131" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="134"/>
-      <c r="D11" s="134"/>
-      <c r="E11" s="135"/>
-      <c r="F11" s="139" t="s">
+      <c r="C11" s="132"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="140"/>
-      <c r="H11" s="140"/>
-      <c r="I11" s="140"/>
-      <c r="J11" s="140"/>
-      <c r="K11" s="141"/>
+      <c r="G11" s="138"/>
+      <c r="H11" s="138"/>
+      <c r="I11" s="138"/>
+      <c r="J11" s="138"/>
+      <c r="K11" s="139"/>
       <c r="L11" s="9"/>
       <c r="N11" s="3"/>
-      <c r="O11" s="145" t="s">
+      <c r="O11" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="P11" s="146"/>
-      <c r="Q11" s="147"/>
-      <c r="R11" s="145" t="s">
+      <c r="P11" s="144"/>
+      <c r="Q11" s="145"/>
+      <c r="R11" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="S11" s="146"/>
-      <c r="T11" s="147"/>
-      <c r="U11" s="145" t="s">
+      <c r="S11" s="144"/>
+      <c r="T11" s="145"/>
+      <c r="U11" s="143" t="s">
         <v>13</v>
       </c>
-      <c r="V11" s="146"/>
-      <c r="W11" s="151"/>
+      <c r="V11" s="144"/>
+      <c r="W11" s="149"/>
       <c r="X11" s="3"/>
     </row>
     <row r="12" spans="1:24" ht="43.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="136"/>
-      <c r="C12" s="137"/>
-      <c r="D12" s="137"/>
-      <c r="E12" s="138"/>
-      <c r="F12" s="142"/>
-      <c r="G12" s="143"/>
-      <c r="H12" s="143"/>
-      <c r="I12" s="143"/>
-      <c r="J12" s="143"/>
-      <c r="K12" s="144"/>
+      <c r="B12" s="134"/>
+      <c r="C12" s="135"/>
+      <c r="D12" s="135"/>
+      <c r="E12" s="136"/>
+      <c r="F12" s="140"/>
+      <c r="G12" s="141"/>
+      <c r="H12" s="141"/>
+      <c r="I12" s="141"/>
+      <c r="J12" s="141"/>
+      <c r="K12" s="142"/>
       <c r="L12" s="9"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="148"/>
-      <c r="P12" s="149"/>
-      <c r="Q12" s="150"/>
-      <c r="R12" s="148"/>
-      <c r="S12" s="149"/>
-      <c r="T12" s="150"/>
-      <c r="U12" s="148"/>
-      <c r="V12" s="149"/>
-      <c r="W12" s="152"/>
+      <c r="O12" s="146"/>
+      <c r="P12" s="147"/>
+      <c r="Q12" s="148"/>
+      <c r="R12" s="146"/>
+      <c r="S12" s="147"/>
+      <c r="T12" s="148"/>
+      <c r="U12" s="146"/>
+      <c r="V12" s="147"/>
+      <c r="W12" s="150"/>
       <c r="X12" s="3"/>
     </row>
-    <row r="13" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="171"/>
-      <c r="C13" s="172"/>
-      <c r="D13" s="172"/>
-      <c r="E13" s="172"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="102"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="103"/>
+      <c r="B13" s="205"/>
+      <c r="C13" s="206"/>
+      <c r="D13" s="206"/>
+      <c r="E13" s="206"/>
+      <c r="F13" s="220"/>
+      <c r="G13" s="221"/>
+      <c r="H13" s="221"/>
+      <c r="I13" s="221"/>
+      <c r="J13" s="221"/>
+      <c r="K13" s="222"/>
       <c r="L13" s="9"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="203"/>
-      <c r="P13" s="204"/>
-      <c r="Q13" s="205"/>
-      <c r="R13" s="206"/>
-      <c r="S13" s="204"/>
-      <c r="T13" s="205"/>
-      <c r="U13" s="207"/>
-      <c r="V13" s="208"/>
-      <c r="W13" s="209"/>
+      <c r="O13" s="153"/>
+      <c r="P13" s="154"/>
+      <c r="Q13" s="155"/>
+      <c r="R13" s="187"/>
+      <c r="S13" s="154"/>
+      <c r="T13" s="155"/>
+      <c r="U13" s="163"/>
+      <c r="V13" s="164"/>
+      <c r="W13" s="165"/>
       <c r="X13" s="3"/>
     </row>
-    <row r="14" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="110"/>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="104"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="105"/>
-      <c r="I14" s="105"/>
-      <c r="J14" s="105"/>
-      <c r="K14" s="106"/>
+      <c r="B14" s="207"/>
+      <c r="C14" s="208"/>
+      <c r="D14" s="208"/>
+      <c r="E14" s="209"/>
+      <c r="F14" s="223"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="102"/>
+      <c r="J14" s="102"/>
+      <c r="K14" s="103"/>
       <c r="L14" s="9"/>
       <c r="N14" s="3"/>
-      <c r="O14" s="210"/>
-      <c r="P14" s="211"/>
-      <c r="Q14" s="212"/>
-      <c r="R14" s="213"/>
-      <c r="S14" s="211"/>
-      <c r="T14" s="212"/>
-      <c r="U14" s="214"/>
-      <c r="V14" s="215"/>
-      <c r="W14" s="216"/>
+      <c r="O14" s="95"/>
+      <c r="P14" s="96"/>
+      <c r="Q14" s="97"/>
+      <c r="R14" s="101"/>
+      <c r="S14" s="96"/>
+      <c r="T14" s="97"/>
+      <c r="U14" s="166"/>
+      <c r="V14" s="167"/>
+      <c r="W14" s="168"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="110"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="107"/>
-      <c r="G15" s="108"/>
-      <c r="H15" s="108"/>
-      <c r="I15" s="108"/>
-      <c r="J15" s="108"/>
-      <c r="K15" s="109"/>
+      <c r="B15" s="207"/>
+      <c r="C15" s="208"/>
+      <c r="D15" s="208"/>
+      <c r="E15" s="209"/>
+      <c r="F15" s="224"/>
+      <c r="G15" s="225"/>
+      <c r="H15" s="225"/>
+      <c r="I15" s="225"/>
+      <c r="J15" s="225"/>
+      <c r="K15" s="226"/>
       <c r="L15" s="9"/>
       <c r="N15" s="3"/>
-      <c r="O15" s="210"/>
-      <c r="P15" s="211"/>
-      <c r="Q15" s="212"/>
-      <c r="R15" s="213"/>
-      <c r="S15" s="211"/>
-      <c r="T15" s="212"/>
-      <c r="U15" s="214"/>
-      <c r="V15" s="215"/>
-      <c r="W15" s="216"/>
+      <c r="O15" s="95"/>
+      <c r="P15" s="96"/>
+      <c r="Q15" s="97"/>
+      <c r="R15" s="101"/>
+      <c r="S15" s="96"/>
+      <c r="T15" s="97"/>
+      <c r="U15" s="166"/>
+      <c r="V15" s="167"/>
+      <c r="W15" s="168"/>
       <c r="X15" s="3"/>
     </row>
-    <row r="16" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="162"/>
-      <c r="C16" s="163"/>
-      <c r="D16" s="163"/>
-      <c r="E16" s="164"/>
-      <c r="F16" s="104"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="105"/>
-      <c r="J16" s="105"/>
-      <c r="K16" s="106"/>
+      <c r="B16" s="207"/>
+      <c r="C16" s="208"/>
+      <c r="D16" s="208"/>
+      <c r="E16" s="209"/>
+      <c r="F16" s="223"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="102"/>
+      <c r="I16" s="102"/>
+      <c r="J16" s="102"/>
+      <c r="K16" s="103"/>
       <c r="L16" s="9"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="210"/>
-      <c r="P16" s="211"/>
-      <c r="Q16" s="212"/>
-      <c r="R16" s="213"/>
-      <c r="S16" s="211"/>
-      <c r="T16" s="212"/>
-      <c r="U16" s="214"/>
-      <c r="V16" s="215"/>
-      <c r="W16" s="216"/>
+      <c r="O16" s="95"/>
+      <c r="P16" s="96"/>
+      <c r="Q16" s="97"/>
+      <c r="R16" s="101"/>
+      <c r="S16" s="96"/>
+      <c r="T16" s="97"/>
+      <c r="U16" s="166"/>
+      <c r="V16" s="167"/>
+      <c r="W16" s="168"/>
       <c r="X16" s="3"/>
     </row>
-    <row r="17" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="173"/>
-      <c r="C17" s="174"/>
-      <c r="D17" s="174"/>
-      <c r="E17" s="175"/>
-      <c r="F17" s="104"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="105"/>
-      <c r="I17" s="105"/>
-      <c r="J17" s="105"/>
-      <c r="K17" s="106"/>
+      <c r="B17" s="105"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="223"/>
+      <c r="G17" s="102"/>
+      <c r="H17" s="102"/>
+      <c r="I17" s="102"/>
+      <c r="J17" s="102"/>
+      <c r="K17" s="103"/>
       <c r="L17" s="9"/>
       <c r="N17" s="3"/>
-      <c r="O17" s="210"/>
-      <c r="P17" s="211"/>
-      <c r="Q17" s="212"/>
-      <c r="R17" s="213"/>
-      <c r="S17" s="211"/>
-      <c r="T17" s="212"/>
-      <c r="U17" s="214"/>
-      <c r="V17" s="215"/>
-      <c r="W17" s="216"/>
+      <c r="O17" s="95"/>
+      <c r="P17" s="96"/>
+      <c r="Q17" s="97"/>
+      <c r="R17" s="101"/>
+      <c r="S17" s="96"/>
+      <c r="T17" s="97"/>
+      <c r="U17" s="166"/>
+      <c r="V17" s="167"/>
+      <c r="W17" s="168"/>
       <c r="X17" s="3"/>
     </row>
-    <row r="18" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="165"/>
-      <c r="C18" s="166"/>
-      <c r="D18" s="166"/>
-      <c r="E18" s="167"/>
-      <c r="F18" s="107"/>
-      <c r="G18" s="108"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="108"/>
-      <c r="J18" s="108"/>
-      <c r="K18" s="109"/>
+      <c r="B18" s="210"/>
+      <c r="C18" s="211"/>
+      <c r="D18" s="211"/>
+      <c r="E18" s="212"/>
+      <c r="F18" s="224"/>
+      <c r="G18" s="225"/>
+      <c r="H18" s="225"/>
+      <c r="I18" s="225"/>
+      <c r="J18" s="225"/>
+      <c r="K18" s="226"/>
       <c r="L18" s="9"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="210"/>
-      <c r="P18" s="211"/>
-      <c r="Q18" s="212"/>
-      <c r="R18" s="213"/>
-      <c r="S18" s="211"/>
-      <c r="T18" s="212"/>
-      <c r="U18" s="214"/>
-      <c r="V18" s="215"/>
-      <c r="W18" s="216"/>
+      <c r="O18" s="95"/>
+      <c r="P18" s="96"/>
+      <c r="Q18" s="97"/>
+      <c r="R18" s="101"/>
+      <c r="S18" s="96"/>
+      <c r="T18" s="97"/>
+      <c r="U18" s="166"/>
+      <c r="V18" s="167"/>
+      <c r="W18" s="168"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="165"/>
-      <c r="C19" s="166"/>
-      <c r="D19" s="166"/>
-      <c r="E19" s="167"/>
-      <c r="F19" s="104"/>
-      <c r="G19" s="105"/>
-      <c r="H19" s="105"/>
-      <c r="I19" s="105"/>
-      <c r="J19" s="105"/>
-      <c r="K19" s="106"/>
+      <c r="B19" s="210"/>
+      <c r="C19" s="211"/>
+      <c r="D19" s="211"/>
+      <c r="E19" s="212"/>
+      <c r="F19" s="223"/>
+      <c r="G19" s="102"/>
+      <c r="H19" s="102"/>
+      <c r="I19" s="102"/>
+      <c r="J19" s="102"/>
+      <c r="K19" s="103"/>
       <c r="L19" s="9"/>
       <c r="N19" s="3"/>
-      <c r="O19" s="210"/>
-      <c r="P19" s="211"/>
-      <c r="Q19" s="212"/>
-      <c r="R19" s="213"/>
-      <c r="S19" s="211"/>
-      <c r="T19" s="212"/>
-      <c r="U19" s="214"/>
-      <c r="V19" s="215"/>
-      <c r="W19" s="216"/>
+      <c r="O19" s="95"/>
+      <c r="P19" s="96"/>
+      <c r="Q19" s="97"/>
+      <c r="R19" s="101"/>
+      <c r="S19" s="96"/>
+      <c r="T19" s="97"/>
+      <c r="U19" s="166"/>
+      <c r="V19" s="167"/>
+      <c r="W19" s="168"/>
       <c r="X19" s="3"/>
     </row>
-    <row r="20" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="165"/>
-      <c r="C20" s="166"/>
-      <c r="D20" s="166"/>
-      <c r="E20" s="167"/>
-      <c r="F20" s="104"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="105"/>
-      <c r="I20" s="105"/>
-      <c r="J20" s="105"/>
-      <c r="K20" s="106"/>
+      <c r="B20" s="210"/>
+      <c r="C20" s="211"/>
+      <c r="D20" s="211"/>
+      <c r="E20" s="212"/>
+      <c r="F20" s="223"/>
+      <c r="G20" s="102"/>
+      <c r="H20" s="102"/>
+      <c r="I20" s="102"/>
+      <c r="J20" s="102"/>
+      <c r="K20" s="103"/>
       <c r="L20" s="9"/>
       <c r="N20" s="3"/>
-      <c r="O20" s="210"/>
-      <c r="P20" s="211"/>
-      <c r="Q20" s="212"/>
-      <c r="R20" s="213"/>
-      <c r="S20" s="211"/>
-      <c r="T20" s="212"/>
-      <c r="U20" s="214"/>
-      <c r="V20" s="215"/>
-      <c r="W20" s="216"/>
+      <c r="O20" s="95"/>
+      <c r="P20" s="96"/>
+      <c r="Q20" s="97"/>
+      <c r="R20" s="101"/>
+      <c r="S20" s="96"/>
+      <c r="T20" s="97"/>
+      <c r="U20" s="166"/>
+      <c r="V20" s="167"/>
+      <c r="W20" s="168"/>
       <c r="X20" s="3"/>
     </row>
     <row r="21" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="165"/>
-      <c r="C21" s="166"/>
-      <c r="D21" s="166"/>
-      <c r="E21" s="167"/>
-      <c r="F21" s="107"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="108"/>
-      <c r="I21" s="108"/>
-      <c r="J21" s="108"/>
-      <c r="K21" s="109"/>
+      <c r="B21" s="210"/>
+      <c r="C21" s="211"/>
+      <c r="D21" s="211"/>
+      <c r="E21" s="212"/>
+      <c r="F21" s="224"/>
+      <c r="G21" s="225"/>
+      <c r="H21" s="225"/>
+      <c r="I21" s="225"/>
+      <c r="J21" s="225"/>
+      <c r="K21" s="226"/>
       <c r="L21" s="9"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="210"/>
-      <c r="P21" s="211"/>
-      <c r="Q21" s="212"/>
-      <c r="R21" s="213"/>
-      <c r="S21" s="211"/>
-      <c r="T21" s="212"/>
-      <c r="U21" s="214"/>
-      <c r="V21" s="215"/>
-      <c r="W21" s="216"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="96"/>
+      <c r="Q21" s="97"/>
+      <c r="R21" s="101"/>
+      <c r="S21" s="96"/>
+      <c r="T21" s="97"/>
+      <c r="U21" s="166"/>
+      <c r="V21" s="167"/>
+      <c r="W21" s="168"/>
       <c r="X21" s="3"/>
     </row>
     <row r="22" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="165"/>
-      <c r="C22" s="166"/>
-      <c r="D22" s="166"/>
-      <c r="E22" s="167"/>
-      <c r="F22" s="104"/>
-      <c r="G22" s="105"/>
-      <c r="H22" s="105"/>
-      <c r="I22" s="105"/>
-      <c r="J22" s="105"/>
-      <c r="K22" s="106"/>
+      <c r="B22" s="210"/>
+      <c r="C22" s="211"/>
+      <c r="D22" s="211"/>
+      <c r="E22" s="212"/>
+      <c r="F22" s="223"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="102"/>
+      <c r="I22" s="102"/>
+      <c r="J22" s="102"/>
+      <c r="K22" s="103"/>
       <c r="L22" s="9"/>
       <c r="N22" s="3"/>
-      <c r="O22" s="210"/>
-      <c r="P22" s="211"/>
-      <c r="Q22" s="212"/>
-      <c r="R22" s="213"/>
-      <c r="S22" s="211"/>
-      <c r="T22" s="212"/>
-      <c r="U22" s="214"/>
-      <c r="V22" s="215"/>
-      <c r="W22" s="216"/>
+      <c r="O22" s="95"/>
+      <c r="P22" s="96"/>
+      <c r="Q22" s="97"/>
+      <c r="R22" s="101"/>
+      <c r="S22" s="96"/>
+      <c r="T22" s="97"/>
+      <c r="U22" s="166"/>
+      <c r="V22" s="167"/>
+      <c r="W22" s="168"/>
       <c r="X22" s="3"/>
     </row>
     <row r="23" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="123"/>
-      <c r="C23" s="124"/>
-      <c r="D23" s="124"/>
-      <c r="E23" s="125"/>
-      <c r="F23" s="107"/>
-      <c r="G23" s="108"/>
-      <c r="H23" s="108"/>
-      <c r="I23" s="108"/>
-      <c r="J23" s="108"/>
-      <c r="K23" s="109"/>
+      <c r="B23" s="213"/>
+      <c r="C23" s="214"/>
+      <c r="D23" s="214"/>
+      <c r="E23" s="215"/>
+      <c r="F23" s="224"/>
+      <c r="G23" s="225"/>
+      <c r="H23" s="225"/>
+      <c r="I23" s="225"/>
+      <c r="J23" s="225"/>
+      <c r="K23" s="226"/>
       <c r="L23" s="9"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="210"/>
-      <c r="P23" s="211"/>
-      <c r="Q23" s="212"/>
-      <c r="R23" s="213"/>
-      <c r="S23" s="211"/>
-      <c r="T23" s="212"/>
-      <c r="U23" s="214"/>
-      <c r="V23" s="215"/>
-      <c r="W23" s="216"/>
+      <c r="O23" s="95"/>
+      <c r="P23" s="96"/>
+      <c r="Q23" s="97"/>
+      <c r="R23" s="101"/>
+      <c r="S23" s="96"/>
+      <c r="T23" s="97"/>
+      <c r="U23" s="166"/>
+      <c r="V23" s="167"/>
+      <c r="W23" s="168"/>
       <c r="X23" s="3"/>
     </row>
     <row r="24" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="123"/>
-      <c r="C24" s="124"/>
-      <c r="D24" s="124"/>
-      <c r="E24" s="125"/>
-      <c r="F24" s="104"/>
-      <c r="G24" s="105"/>
-      <c r="H24" s="105"/>
-      <c r="I24" s="105"/>
-      <c r="J24" s="105"/>
-      <c r="K24" s="106"/>
+      <c r="B24" s="213"/>
+      <c r="C24" s="214"/>
+      <c r="D24" s="214"/>
+      <c r="E24" s="215"/>
+      <c r="F24" s="223"/>
+      <c r="G24" s="102"/>
+      <c r="H24" s="102"/>
+      <c r="I24" s="102"/>
+      <c r="J24" s="102"/>
+      <c r="K24" s="103"/>
       <c r="L24" s="9"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="210"/>
-      <c r="P24" s="211"/>
-      <c r="Q24" s="212"/>
-      <c r="R24" s="213"/>
-      <c r="S24" s="211"/>
-      <c r="T24" s="212"/>
-      <c r="U24" s="214"/>
-      <c r="V24" s="215"/>
-      <c r="W24" s="216"/>
+      <c r="O24" s="95"/>
+      <c r="P24" s="96"/>
+      <c r="Q24" s="97"/>
+      <c r="R24" s="101"/>
+      <c r="S24" s="96"/>
+      <c r="T24" s="97"/>
+      <c r="U24" s="166"/>
+      <c r="V24" s="167"/>
+      <c r="W24" s="168"/>
       <c r="X24" s="3"/>
     </row>
     <row r="25" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="123"/>
-      <c r="C25" s="124"/>
-      <c r="D25" s="124"/>
-      <c r="E25" s="125"/>
-      <c r="F25" s="104"/>
-      <c r="G25" s="105"/>
-      <c r="H25" s="105"/>
-      <c r="I25" s="105"/>
-      <c r="J25" s="105"/>
-      <c r="K25" s="106"/>
+      <c r="B25" s="213"/>
+      <c r="C25" s="214"/>
+      <c r="D25" s="214"/>
+      <c r="E25" s="215"/>
+      <c r="F25" s="223"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="102"/>
+      <c r="I25" s="102"/>
+      <c r="J25" s="102"/>
+      <c r="K25" s="103"/>
       <c r="L25" s="9"/>
       <c r="N25" s="3"/>
-      <c r="O25" s="210"/>
-      <c r="P25" s="211"/>
-      <c r="Q25" s="212"/>
-      <c r="R25" s="213"/>
-      <c r="S25" s="211"/>
-      <c r="T25" s="212"/>
-      <c r="U25" s="214"/>
-      <c r="V25" s="215"/>
-      <c r="W25" s="216"/>
+      <c r="O25" s="95"/>
+      <c r="P25" s="96"/>
+      <c r="Q25" s="97"/>
+      <c r="R25" s="101"/>
+      <c r="S25" s="96"/>
+      <c r="T25" s="97"/>
+      <c r="U25" s="166"/>
+      <c r="V25" s="167"/>
+      <c r="W25" s="168"/>
       <c r="X25" s="3"/>
     </row>
     <row r="26" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="123"/>
-      <c r="C26" s="124"/>
-      <c r="D26" s="124"/>
-      <c r="E26" s="125"/>
-      <c r="F26" s="107"/>
-      <c r="G26" s="108"/>
-      <c r="H26" s="108"/>
-      <c r="I26" s="108"/>
-      <c r="J26" s="108"/>
-      <c r="K26" s="109"/>
+      <c r="B26" s="213"/>
+      <c r="C26" s="214"/>
+      <c r="D26" s="214"/>
+      <c r="E26" s="215"/>
+      <c r="F26" s="224"/>
+      <c r="G26" s="225"/>
+      <c r="H26" s="225"/>
+      <c r="I26" s="225"/>
+      <c r="J26" s="225"/>
+      <c r="K26" s="226"/>
       <c r="L26" s="9"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="210"/>
-      <c r="P26" s="211"/>
-      <c r="Q26" s="212"/>
-      <c r="R26" s="213"/>
-      <c r="S26" s="211"/>
-      <c r="T26" s="212"/>
-      <c r="U26" s="214"/>
-      <c r="V26" s="215"/>
-      <c r="W26" s="216"/>
+      <c r="O26" s="95"/>
+      <c r="P26" s="96"/>
+      <c r="Q26" s="97"/>
+      <c r="R26" s="101"/>
+      <c r="S26" s="96"/>
+      <c r="T26" s="97"/>
+      <c r="U26" s="166"/>
+      <c r="V26" s="167"/>
+      <c r="W26" s="168"/>
       <c r="X26" s="3"/>
     </row>
     <row r="27" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="168"/>
-      <c r="C27" s="169"/>
-      <c r="D27" s="169"/>
-      <c r="E27" s="170"/>
-      <c r="F27" s="159"/>
-      <c r="G27" s="160"/>
-      <c r="H27" s="160"/>
-      <c r="I27" s="160"/>
-      <c r="J27" s="160"/>
-      <c r="K27" s="161"/>
+      <c r="B27" s="216"/>
+      <c r="C27" s="217"/>
+      <c r="D27" s="217"/>
+      <c r="E27" s="218"/>
+      <c r="F27" s="227"/>
+      <c r="G27" s="228"/>
+      <c r="H27" s="228"/>
+      <c r="I27" s="228"/>
+      <c r="J27" s="228"/>
+      <c r="K27" s="229"/>
       <c r="L27" s="9"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="217"/>
-      <c r="P27" s="218"/>
-      <c r="Q27" s="219"/>
-      <c r="R27" s="220"/>
-      <c r="S27" s="218"/>
-      <c r="T27" s="219"/>
-      <c r="U27" s="221"/>
-      <c r="V27" s="222"/>
-      <c r="W27" s="223"/>
+      <c r="O27" s="98"/>
+      <c r="P27" s="99"/>
+      <c r="Q27" s="100"/>
+      <c r="R27" s="104"/>
+      <c r="S27" s="99"/>
+      <c r="T27" s="100"/>
+      <c r="U27" s="188"/>
+      <c r="V27" s="189"/>
+      <c r="W27" s="190"/>
       <c r="X27" s="3"/>
     </row>
     <row r="28" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="61"/>
-      <c r="J28" s="61"/>
-      <c r="K28" s="61"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="62"/>
       <c r="L28" s="9"/>
       <c r="N28" s="3"/>
-      <c r="O28" s="58"/>
-      <c r="P28" s="58"/>
-      <c r="Q28" s="58"/>
-      <c r="R28" s="58"/>
-      <c r="S28" s="58"/>
-      <c r="T28" s="58"/>
-      <c r="U28" s="58"/>
-      <c r="V28" s="58"/>
-      <c r="W28" s="66"/>
+      <c r="O28" s="180"/>
+      <c r="P28" s="180"/>
+      <c r="Q28" s="180"/>
+      <c r="R28" s="180"/>
+      <c r="S28" s="180"/>
+      <c r="T28" s="180"/>
+      <c r="U28" s="180"/>
+      <c r="V28" s="180"/>
+      <c r="W28" s="186"/>
       <c r="X28" s="3"/>
     </row>
     <row r="29" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="197" t="s">
+      <c r="B29" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="198"/>
-      <c r="D29" s="198"/>
-      <c r="E29" s="198"/>
-      <c r="F29" s="198"/>
-      <c r="G29" s="198"/>
-      <c r="H29" s="198"/>
-      <c r="I29" s="198"/>
-      <c r="J29" s="198"/>
-      <c r="K29" s="28"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="27"/>
       <c r="L29" s="9"/>
       <c r="N29" s="3"/>
-      <c r="O29" s="200" t="s">
+      <c r="O29" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="P29" s="201"/>
-      <c r="Q29" s="201"/>
-      <c r="R29" s="201"/>
-      <c r="S29" s="201"/>
-      <c r="T29" s="201"/>
-      <c r="U29" s="201"/>
-      <c r="V29" s="201"/>
-      <c r="W29" s="201"/>
+      <c r="P29" s="60"/>
+      <c r="Q29" s="60"/>
+      <c r="R29" s="60"/>
+      <c r="S29" s="60"/>
+      <c r="T29" s="60"/>
+      <c r="U29" s="60"/>
+      <c r="V29" s="60"/>
+      <c r="W29" s="60"/>
       <c r="X29" s="3"/>
     </row>
     <row r="30" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" s="199"/>
-      <c r="C30" s="199"/>
-      <c r="D30" s="199"/>
-      <c r="E30" s="199"/>
-      <c r="F30" s="199"/>
-      <c r="G30" s="199"/>
-      <c r="H30" s="199"/>
-      <c r="I30" s="199"/>
-      <c r="J30" s="199"/>
-      <c r="K30" s="27"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="26"/>
       <c r="L30" s="9"/>
       <c r="N30" s="3"/>
-      <c r="O30" s="202"/>
-      <c r="P30" s="202"/>
-      <c r="Q30" s="202"/>
-      <c r="R30" s="202"/>
-      <c r="S30" s="202"/>
-      <c r="T30" s="202"/>
-      <c r="U30" s="202"/>
-      <c r="V30" s="202"/>
-      <c r="W30" s="202"/>
+      <c r="O30" s="61"/>
+      <c r="P30" s="61"/>
+      <c r="Q30" s="61"/>
+      <c r="R30" s="61"/>
+      <c r="S30" s="61"/>
+      <c r="T30" s="61"/>
+      <c r="U30" s="61"/>
+      <c r="V30" s="61"/>
+      <c r="W30" s="61"/>
       <c r="X30" s="3"/>
     </row>
     <row r="31" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
-      <c r="B31" s="184" t="s">
+      <c r="B31" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="185"/>
-      <c r="D31" s="184" t="s">
+      <c r="C31" s="81"/>
+      <c r="D31" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="188"/>
-      <c r="F31" s="185"/>
-      <c r="G31" s="184" t="s">
+      <c r="E31" s="84"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="H31" s="188"/>
-      <c r="I31" s="188"/>
-      <c r="J31" s="185"/>
-      <c r="K31" s="193" t="s">
+      <c r="H31" s="84"/>
+      <c r="I31" s="84"/>
+      <c r="J31" s="81"/>
+      <c r="K31" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="L31" s="26"/>
-      <c r="M31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="24"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="176" t="s">
+      <c r="O31" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="P31" s="176"/>
-      <c r="Q31" s="176"/>
-      <c r="R31" s="176" t="s">
+      <c r="P31" s="63"/>
+      <c r="Q31" s="63"/>
+      <c r="R31" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="S31" s="176"/>
-      <c r="T31" s="176"/>
-      <c r="U31" s="176"/>
-      <c r="V31" s="176"/>
-      <c r="W31" s="177"/>
+      <c r="S31" s="63"/>
+      <c r="T31" s="63"/>
+      <c r="U31" s="63"/>
+      <c r="V31" s="63"/>
+      <c r="W31" s="64"/>
       <c r="X31" s="3"/>
     </row>
     <row r="32" spans="1:24" ht="43.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
-      <c r="B32" s="186"/>
-      <c r="C32" s="187"/>
-      <c r="D32" s="189"/>
-      <c r="E32" s="190"/>
-      <c r="F32" s="191"/>
-      <c r="G32" s="186"/>
-      <c r="H32" s="192"/>
-      <c r="I32" s="192"/>
-      <c r="J32" s="187"/>
-      <c r="K32" s="194"/>
+      <c r="B32" s="82"/>
+      <c r="C32" s="83"/>
+      <c r="D32" s="85"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="82"/>
+      <c r="H32" s="88"/>
+      <c r="I32" s="88"/>
+      <c r="J32" s="83"/>
+      <c r="K32" s="90"/>
       <c r="L32" s="9"/>
       <c r="N32" s="3"/>
-      <c r="O32" s="176"/>
-      <c r="P32" s="176"/>
-      <c r="Q32" s="176"/>
-      <c r="R32" s="176"/>
-      <c r="S32" s="176"/>
-      <c r="T32" s="176"/>
-      <c r="U32" s="176"/>
-      <c r="V32" s="176"/>
-      <c r="W32" s="177"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="63"/>
+      <c r="Q32" s="63"/>
+      <c r="R32" s="63"/>
+      <c r="S32" s="63"/>
+      <c r="T32" s="63"/>
+      <c r="U32" s="63"/>
+      <c r="V32" s="63"/>
+      <c r="W32" s="64"/>
       <c r="X32" s="3"/>
     </row>
-    <row r="33" spans="1:24" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" ht="149.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="19">
         <v>1</v>
       </c>
-      <c r="C33" s="24"/>
+      <c r="C33" s="219"/>
       <c r="D33" s="20"/>
-      <c r="E33" s="195"/>
-      <c r="F33" s="196"/>
+      <c r="E33" s="91"/>
+      <c r="F33" s="92"/>
       <c r="G33" s="18"/>
       <c r="H33" s="17"/>
       <c r="I33" s="16"/>
@@ -5777,24 +5789,24 @@
       <c r="K33" s="14"/>
       <c r="L33" s="9"/>
       <c r="N33" s="3"/>
-      <c r="O33" s="224"/>
-      <c r="P33" s="225"/>
-      <c r="Q33" s="226"/>
-      <c r="R33" s="224"/>
-      <c r="S33" s="225"/>
-      <c r="T33" s="225"/>
-      <c r="U33" s="225"/>
-      <c r="V33" s="225"/>
-      <c r="W33" s="227"/>
+      <c r="O33" s="194"/>
+      <c r="P33" s="195"/>
+      <c r="Q33" s="196"/>
+      <c r="R33" s="194"/>
+      <c r="S33" s="195"/>
+      <c r="T33" s="195"/>
+      <c r="U33" s="195"/>
+      <c r="V33" s="195"/>
+      <c r="W33" s="197"/>
       <c r="X33" s="3"/>
     </row>
     <row r="34" spans="1:24" ht="43.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="19"/>
       <c r="C34" s="23"/>
-      <c r="D34" s="111"/>
-      <c r="E34" s="112"/>
-      <c r="F34" s="113"/>
+      <c r="D34" s="114"/>
+      <c r="E34" s="115"/>
+      <c r="F34" s="116"/>
       <c r="G34" s="18"/>
       <c r="H34" s="17"/>
       <c r="I34" s="16"/>
@@ -5802,26 +5814,26 @@
       <c r="K34" s="22"/>
       <c r="L34" s="9"/>
       <c r="N34" s="3"/>
-      <c r="O34" s="224"/>
-      <c r="P34" s="225"/>
-      <c r="Q34" s="226"/>
-      <c r="R34" s="224"/>
-      <c r="S34" s="225"/>
-      <c r="T34" s="225"/>
-      <c r="U34" s="225"/>
-      <c r="V34" s="225"/>
-      <c r="W34" s="227"/>
+      <c r="O34" s="194"/>
+      <c r="P34" s="195"/>
+      <c r="Q34" s="196"/>
+      <c r="R34" s="194"/>
+      <c r="S34" s="195"/>
+      <c r="T34" s="195"/>
+      <c r="U34" s="195"/>
+      <c r="V34" s="195"/>
+      <c r="W34" s="197"/>
       <c r="X34" s="3"/>
     </row>
-    <row r="35" spans="1:24" ht="108.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="19">
         <v>2</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="20"/>
-      <c r="E35" s="117"/>
-      <c r="F35" s="118"/>
+      <c r="E35" s="93"/>
+      <c r="F35" s="94"/>
       <c r="G35" s="18"/>
       <c r="H35" s="17"/>
       <c r="I35" s="16"/>
@@ -5829,24 +5841,24 @@
       <c r="K35" s="14"/>
       <c r="L35" s="9"/>
       <c r="N35" s="3"/>
-      <c r="O35" s="224"/>
-      <c r="P35" s="225"/>
-      <c r="Q35" s="226"/>
-      <c r="R35" s="224"/>
-      <c r="S35" s="225"/>
-      <c r="T35" s="225"/>
-      <c r="U35" s="225"/>
-      <c r="V35" s="225"/>
-      <c r="W35" s="227"/>
+      <c r="O35" s="194"/>
+      <c r="P35" s="195"/>
+      <c r="Q35" s="196"/>
+      <c r="R35" s="194"/>
+      <c r="S35" s="195"/>
+      <c r="T35" s="195"/>
+      <c r="U35" s="195"/>
+      <c r="V35" s="195"/>
+      <c r="W35" s="197"/>
       <c r="X35" s="3"/>
     </row>
     <row r="36" spans="1:24" ht="43.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="19"/>
       <c r="C36" s="23"/>
-      <c r="D36" s="111"/>
-      <c r="E36" s="112"/>
-      <c r="F36" s="113"/>
+      <c r="D36" s="114"/>
+      <c r="E36" s="115"/>
+      <c r="F36" s="116"/>
       <c r="G36" s="18"/>
       <c r="H36" s="17"/>
       <c r="I36" s="16"/>
@@ -5854,26 +5866,26 @@
       <c r="K36" s="22"/>
       <c r="L36" s="9"/>
       <c r="N36" s="3"/>
-      <c r="O36" s="224"/>
-      <c r="P36" s="225"/>
-      <c r="Q36" s="226"/>
-      <c r="R36" s="224"/>
-      <c r="S36" s="225"/>
-      <c r="T36" s="225"/>
-      <c r="U36" s="225"/>
-      <c r="V36" s="225"/>
-      <c r="W36" s="227"/>
+      <c r="O36" s="194"/>
+      <c r="P36" s="195"/>
+      <c r="Q36" s="196"/>
+      <c r="R36" s="194"/>
+      <c r="S36" s="195"/>
+      <c r="T36" s="195"/>
+      <c r="U36" s="195"/>
+      <c r="V36" s="195"/>
+      <c r="W36" s="197"/>
       <c r="X36" s="3"/>
     </row>
-    <row r="37" spans="1:24" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" ht="150.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="19">
         <v>3</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="20"/>
-      <c r="E37" s="117"/>
-      <c r="F37" s="118"/>
+      <c r="E37" s="93"/>
+      <c r="F37" s="94"/>
       <c r="G37" s="18"/>
       <c r="H37" s="17"/>
       <c r="I37" s="16"/>
@@ -5881,24 +5893,24 @@
       <c r="K37" s="14"/>
       <c r="L37" s="9"/>
       <c r="N37" s="3"/>
-      <c r="O37" s="224"/>
-      <c r="P37" s="225"/>
-      <c r="Q37" s="226"/>
-      <c r="R37" s="224"/>
-      <c r="S37" s="225"/>
-      <c r="T37" s="225"/>
-      <c r="U37" s="225"/>
-      <c r="V37" s="225"/>
-      <c r="W37" s="227"/>
+      <c r="O37" s="194"/>
+      <c r="P37" s="195"/>
+      <c r="Q37" s="196"/>
+      <c r="R37" s="194"/>
+      <c r="S37" s="195"/>
+      <c r="T37" s="195"/>
+      <c r="U37" s="195"/>
+      <c r="V37" s="195"/>
+      <c r="W37" s="197"/>
       <c r="X37" s="3"/>
     </row>
     <row r="38" spans="1:24" ht="43.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="19"/>
       <c r="C38" s="23"/>
-      <c r="D38" s="111"/>
-      <c r="E38" s="112"/>
-      <c r="F38" s="113"/>
+      <c r="D38" s="114"/>
+      <c r="E38" s="115"/>
+      <c r="F38" s="116"/>
       <c r="G38" s="18"/>
       <c r="H38" s="17"/>
       <c r="I38" s="16"/>
@@ -5906,26 +5918,26 @@
       <c r="K38" s="22"/>
       <c r="L38" s="9"/>
       <c r="N38" s="3"/>
-      <c r="O38" s="224"/>
-      <c r="P38" s="225"/>
-      <c r="Q38" s="226"/>
-      <c r="R38" s="224"/>
-      <c r="S38" s="225"/>
-      <c r="T38" s="225"/>
-      <c r="U38" s="225"/>
-      <c r="V38" s="225"/>
-      <c r="W38" s="227"/>
+      <c r="O38" s="194"/>
+      <c r="P38" s="195"/>
+      <c r="Q38" s="196"/>
+      <c r="R38" s="194"/>
+      <c r="S38" s="195"/>
+      <c r="T38" s="195"/>
+      <c r="U38" s="195"/>
+      <c r="V38" s="195"/>
+      <c r="W38" s="197"/>
       <c r="X38" s="3"/>
     </row>
-    <row r="39" spans="1:24" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" ht="150.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="19">
         <v>4</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="20"/>
-      <c r="E39" s="117"/>
-      <c r="F39" s="118"/>
+      <c r="E39" s="93"/>
+      <c r="F39" s="94"/>
       <c r="G39" s="18"/>
       <c r="H39" s="17"/>
       <c r="I39" s="16"/>
@@ -5933,24 +5945,24 @@
       <c r="K39" s="14"/>
       <c r="L39" s="9"/>
       <c r="N39" s="3"/>
-      <c r="O39" s="224"/>
-      <c r="P39" s="225"/>
-      <c r="Q39" s="226"/>
-      <c r="R39" s="224"/>
-      <c r="S39" s="225"/>
-      <c r="T39" s="225"/>
-      <c r="U39" s="225"/>
-      <c r="V39" s="225"/>
-      <c r="W39" s="227"/>
+      <c r="O39" s="194"/>
+      <c r="P39" s="195"/>
+      <c r="Q39" s="196"/>
+      <c r="R39" s="194"/>
+      <c r="S39" s="195"/>
+      <c r="T39" s="195"/>
+      <c r="U39" s="195"/>
+      <c r="V39" s="195"/>
+      <c r="W39" s="197"/>
       <c r="X39" s="3"/>
     </row>
     <row r="40" spans="1:24" ht="43.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="19"/>
       <c r="C40" s="23"/>
-      <c r="D40" s="111"/>
-      <c r="E40" s="112"/>
-      <c r="F40" s="113"/>
+      <c r="D40" s="114"/>
+      <c r="E40" s="115"/>
+      <c r="F40" s="116"/>
       <c r="G40" s="18"/>
       <c r="H40" s="17"/>
       <c r="I40" s="16"/>
@@ -5958,26 +5970,26 @@
       <c r="K40" s="22"/>
       <c r="L40" s="9"/>
       <c r="N40" s="3"/>
-      <c r="O40" s="224"/>
-      <c r="P40" s="225"/>
-      <c r="Q40" s="226"/>
-      <c r="R40" s="224"/>
-      <c r="S40" s="225"/>
-      <c r="T40" s="225"/>
-      <c r="U40" s="225"/>
-      <c r="V40" s="225"/>
-      <c r="W40" s="227"/>
+      <c r="O40" s="194"/>
+      <c r="P40" s="195"/>
+      <c r="Q40" s="196"/>
+      <c r="R40" s="194"/>
+      <c r="S40" s="195"/>
+      <c r="T40" s="195"/>
+      <c r="U40" s="195"/>
+      <c r="V40" s="195"/>
+      <c r="W40" s="197"/>
       <c r="X40" s="3"/>
     </row>
-    <row r="41" spans="1:24" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="19">
         <v>5</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="20"/>
-      <c r="E41" s="114"/>
-      <c r="F41" s="115"/>
+      <c r="E41" s="117"/>
+      <c r="F41" s="118"/>
       <c r="G41" s="18"/>
       <c r="H41" s="17"/>
       <c r="I41" s="16"/>
@@ -5985,24 +5997,24 @@
       <c r="K41" s="14"/>
       <c r="L41" s="9"/>
       <c r="N41" s="3"/>
-      <c r="O41" s="224"/>
-      <c r="P41" s="225"/>
-      <c r="Q41" s="226"/>
-      <c r="R41" s="224"/>
-      <c r="S41" s="225"/>
-      <c r="T41" s="225"/>
-      <c r="U41" s="225"/>
-      <c r="V41" s="225"/>
-      <c r="W41" s="227"/>
+      <c r="O41" s="194"/>
+      <c r="P41" s="195"/>
+      <c r="Q41" s="196"/>
+      <c r="R41" s="194"/>
+      <c r="S41" s="195"/>
+      <c r="T41" s="195"/>
+      <c r="U41" s="195"/>
+      <c r="V41" s="195"/>
+      <c r="W41" s="197"/>
       <c r="X41" s="3"/>
     </row>
     <row r="42" spans="1:24" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="19"/>
       <c r="C42" s="21"/>
-      <c r="D42" s="111"/>
-      <c r="E42" s="112"/>
-      <c r="F42" s="113"/>
+      <c r="D42" s="114"/>
+      <c r="E42" s="115"/>
+      <c r="F42" s="116"/>
       <c r="G42" s="18"/>
       <c r="H42" s="17"/>
       <c r="I42" s="16"/>
@@ -6010,26 +6022,26 @@
       <c r="K42" s="14"/>
       <c r="L42" s="9"/>
       <c r="N42" s="3"/>
-      <c r="O42" s="224"/>
-      <c r="P42" s="225"/>
-      <c r="Q42" s="226"/>
-      <c r="R42" s="224"/>
-      <c r="S42" s="225"/>
-      <c r="T42" s="225"/>
-      <c r="U42" s="225"/>
-      <c r="V42" s="225"/>
-      <c r="W42" s="227"/>
+      <c r="O42" s="194"/>
+      <c r="P42" s="195"/>
+      <c r="Q42" s="196"/>
+      <c r="R42" s="194"/>
+      <c r="S42" s="195"/>
+      <c r="T42" s="195"/>
+      <c r="U42" s="195"/>
+      <c r="V42" s="195"/>
+      <c r="W42" s="197"/>
       <c r="X42" s="3"/>
     </row>
-    <row r="43" spans="1:24" ht="112.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="19">
         <v>6</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="20"/>
-      <c r="E43" s="114"/>
-      <c r="F43" s="115"/>
+      <c r="E43" s="117"/>
+      <c r="F43" s="118"/>
       <c r="G43" s="18"/>
       <c r="H43" s="17"/>
       <c r="I43" s="16"/>
@@ -6037,264 +6049,264 @@
       <c r="K43" s="22"/>
       <c r="L43" s="9"/>
       <c r="N43" s="3"/>
-      <c r="O43" s="224"/>
-      <c r="P43" s="225"/>
-      <c r="Q43" s="226"/>
-      <c r="R43" s="228"/>
-      <c r="S43" s="229"/>
-      <c r="T43" s="229"/>
-      <c r="U43" s="229"/>
-      <c r="V43" s="229"/>
-      <c r="W43" s="230"/>
+      <c r="O43" s="194"/>
+      <c r="P43" s="195"/>
+      <c r="Q43" s="196"/>
+      <c r="R43" s="199"/>
+      <c r="S43" s="200"/>
+      <c r="T43" s="200"/>
+      <c r="U43" s="200"/>
+      <c r="V43" s="200"/>
+      <c r="W43" s="201"/>
       <c r="X43" s="3"/>
     </row>
     <row r="44" spans="1:24" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
-      <c r="B44" s="47"/>
-      <c r="C44" s="48"/>
-      <c r="D44" s="49"/>
-      <c r="E44" s="116"/>
-      <c r="F44" s="116"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="53"/>
-      <c r="K44" s="54"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="198"/>
+      <c r="F44" s="198"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="53"/>
       <c r="M44" s="3"/>
       <c r="N44" s="13"/>
-      <c r="O44" s="74"/>
-      <c r="P44" s="74"/>
-      <c r="Q44" s="74"/>
-      <c r="R44" s="74"/>
-      <c r="S44" s="74"/>
-      <c r="T44" s="74"/>
-      <c r="U44" s="74"/>
-      <c r="V44" s="74"/>
-      <c r="W44" s="74"/>
-      <c r="X44" s="74"/>
+      <c r="O44" s="193"/>
+      <c r="P44" s="193"/>
+      <c r="Q44" s="193"/>
+      <c r="R44" s="193"/>
+      <c r="S44" s="193"/>
+      <c r="T44" s="193"/>
+      <c r="U44" s="193"/>
+      <c r="V44" s="193"/>
+      <c r="W44" s="193"/>
+      <c r="X44" s="193"/>
     </row>
     <row r="45" spans="1:24" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
-      <c r="B45" s="72"/>
-      <c r="C45" s="72"/>
-      <c r="D45" s="72"/>
-      <c r="E45" s="72"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="72"/>
-      <c r="H45" s="72"/>
-      <c r="I45" s="72"/>
-      <c r="J45" s="72"/>
-      <c r="K45" s="72"/>
+      <c r="B45" s="191"/>
+      <c r="C45" s="191"/>
+      <c r="D45" s="191"/>
+      <c r="E45" s="191"/>
+      <c r="F45" s="191"/>
+      <c r="G45" s="191"/>
+      <c r="H45" s="191"/>
+      <c r="I45" s="191"/>
+      <c r="J45" s="191"/>
+      <c r="K45" s="191"/>
       <c r="L45" s="9"/>
       <c r="N45" s="3"/>
-      <c r="O45" s="74"/>
-      <c r="P45" s="74"/>
-      <c r="Q45" s="74"/>
-      <c r="R45" s="74"/>
-      <c r="S45" s="74"/>
-      <c r="T45" s="74"/>
-      <c r="U45" s="74"/>
-      <c r="V45" s="74"/>
-      <c r="W45" s="74"/>
-      <c r="X45" s="74"/>
+      <c r="O45" s="193"/>
+      <c r="P45" s="193"/>
+      <c r="Q45" s="193"/>
+      <c r="R45" s="193"/>
+      <c r="S45" s="193"/>
+      <c r="T45" s="193"/>
+      <c r="U45" s="193"/>
+      <c r="V45" s="193"/>
+      <c r="W45" s="193"/>
+      <c r="X45" s="193"/>
     </row>
     <row r="46" spans="1:24" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
-      <c r="B46" s="73"/>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="73"/>
-      <c r="G46" s="73"/>
-      <c r="H46" s="73"/>
-      <c r="I46" s="73"/>
-      <c r="J46" s="73"/>
-      <c r="K46" s="73"/>
+      <c r="B46" s="192"/>
+      <c r="C46" s="192"/>
+      <c r="D46" s="192"/>
+      <c r="E46" s="192"/>
+      <c r="F46" s="192"/>
+      <c r="G46" s="192"/>
+      <c r="H46" s="192"/>
+      <c r="I46" s="192"/>
+      <c r="J46" s="192"/>
+      <c r="K46" s="192"/>
       <c r="L46" s="9"/>
       <c r="N46" s="3"/>
-      <c r="O46" s="74"/>
-      <c r="P46" s="74"/>
-      <c r="Q46" s="74"/>
-      <c r="R46" s="74"/>
-      <c r="S46" s="74"/>
-      <c r="T46" s="74"/>
-      <c r="U46" s="74"/>
-      <c r="V46" s="74"/>
-      <c r="W46" s="74"/>
-      <c r="X46" s="74"/>
+      <c r="O46" s="193"/>
+      <c r="P46" s="193"/>
+      <c r="Q46" s="193"/>
+      <c r="R46" s="193"/>
+      <c r="S46" s="193"/>
+      <c r="T46" s="193"/>
+      <c r="U46" s="193"/>
+      <c r="V46" s="193"/>
+      <c r="W46" s="193"/>
+      <c r="X46" s="193"/>
     </row>
     <row r="47" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="76" t="s">
+      <c r="C47" s="171" t="s">
         <v>34</v>
       </c>
-      <c r="D47" s="77"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="70"/>
-      <c r="H47" s="78"/>
-      <c r="I47" s="79"/>
-      <c r="J47" s="80"/>
-      <c r="K47" s="81"/>
+      <c r="D47" s="172"/>
+      <c r="E47" s="173"/>
+      <c r="F47" s="174"/>
+      <c r="G47" s="174"/>
+      <c r="H47" s="175"/>
+      <c r="I47" s="176"/>
+      <c r="J47" s="177"/>
+      <c r="K47" s="178"/>
       <c r="L47" s="11"/>
       <c r="M47" s="10"/>
       <c r="N47" s="3"/>
-      <c r="O47" s="55" t="s">
+      <c r="O47" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="P47" s="69"/>
-      <c r="Q47" s="70"/>
-      <c r="R47" s="70"/>
-      <c r="S47" s="70"/>
-      <c r="T47" s="70"/>
-      <c r="U47" s="70"/>
-      <c r="V47" s="70"/>
-      <c r="W47" s="71"/>
+      <c r="P47" s="173"/>
+      <c r="Q47" s="174"/>
+      <c r="R47" s="174"/>
+      <c r="S47" s="174"/>
+      <c r="T47" s="174"/>
+      <c r="U47" s="174"/>
+      <c r="V47" s="174"/>
+      <c r="W47" s="204"/>
       <c r="X47" s="3"/>
     </row>
     <row r="48" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
-      <c r="B48" s="57"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="82" t="s">
+      <c r="B48" s="179"/>
+      <c r="C48" s="180"/>
+      <c r="D48" s="181"/>
+      <c r="E48" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F48" s="83"/>
-      <c r="G48" s="83"/>
-      <c r="H48" s="84"/>
-      <c r="I48" s="82" t="s">
+      <c r="F48" s="66"/>
+      <c r="G48" s="66"/>
+      <c r="H48" s="67"/>
+      <c r="I48" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="J48" s="83"/>
-      <c r="K48" s="84"/>
+      <c r="J48" s="66"/>
+      <c r="K48" s="67"/>
       <c r="L48" s="9"/>
       <c r="N48" s="3"/>
-      <c r="O48" s="57"/>
-      <c r="P48" s="58"/>
-      <c r="Q48" s="59"/>
-      <c r="R48" s="57"/>
-      <c r="S48" s="58"/>
-      <c r="T48" s="59"/>
-      <c r="U48" s="57"/>
-      <c r="V48" s="58"/>
-      <c r="W48" s="66"/>
+      <c r="O48" s="179"/>
+      <c r="P48" s="180"/>
+      <c r="Q48" s="181"/>
+      <c r="R48" s="179"/>
+      <c r="S48" s="180"/>
+      <c r="T48" s="181"/>
+      <c r="U48" s="179"/>
+      <c r="V48" s="180"/>
+      <c r="W48" s="186"/>
       <c r="X48" s="3"/>
     </row>
     <row r="49" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
-      <c r="B49" s="60"/>
-      <c r="C49" s="61"/>
-      <c r="D49" s="62"/>
-      <c r="E49" s="85"/>
-      <c r="F49" s="86"/>
-      <c r="G49" s="86"/>
-      <c r="H49" s="87"/>
-      <c r="I49" s="85"/>
-      <c r="J49" s="86"/>
-      <c r="K49" s="87"/>
+      <c r="B49" s="182"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="123"/>
+      <c r="E49" s="68"/>
+      <c r="F49" s="69"/>
+      <c r="G49" s="69"/>
+      <c r="H49" s="70"/>
+      <c r="I49" s="68"/>
+      <c r="J49" s="69"/>
+      <c r="K49" s="70"/>
       <c r="L49" s="9"/>
       <c r="N49" s="3"/>
-      <c r="O49" s="60"/>
-      <c r="P49" s="61"/>
-      <c r="Q49" s="62"/>
-      <c r="R49" s="60"/>
-      <c r="S49" s="61"/>
-      <c r="T49" s="62"/>
-      <c r="U49" s="60"/>
-      <c r="V49" s="61"/>
-      <c r="W49" s="67"/>
+      <c r="O49" s="182"/>
+      <c r="P49" s="62"/>
+      <c r="Q49" s="123"/>
+      <c r="R49" s="182"/>
+      <c r="S49" s="62"/>
+      <c r="T49" s="123"/>
+      <c r="U49" s="182"/>
+      <c r="V49" s="62"/>
+      <c r="W49" s="202"/>
       <c r="X49" s="3"/>
     </row>
     <row r="50" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
-      <c r="B50" s="60"/>
-      <c r="C50" s="61"/>
-      <c r="D50" s="62"/>
-      <c r="E50" s="85"/>
-      <c r="F50" s="86"/>
-      <c r="G50" s="86"/>
-      <c r="H50" s="87"/>
-      <c r="I50" s="85"/>
-      <c r="J50" s="86"/>
-      <c r="K50" s="87"/>
+      <c r="B50" s="182"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="123"/>
+      <c r="E50" s="68"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="70"/>
+      <c r="I50" s="68"/>
+      <c r="J50" s="69"/>
+      <c r="K50" s="70"/>
       <c r="L50" s="9"/>
       <c r="N50" s="3"/>
-      <c r="O50" s="60"/>
-      <c r="P50" s="61"/>
-      <c r="Q50" s="62"/>
-      <c r="R50" s="60"/>
-      <c r="S50" s="61"/>
-      <c r="T50" s="62"/>
-      <c r="U50" s="60"/>
-      <c r="V50" s="61"/>
-      <c r="W50" s="67"/>
+      <c r="O50" s="182"/>
+      <c r="P50" s="62"/>
+      <c r="Q50" s="123"/>
+      <c r="R50" s="182"/>
+      <c r="S50" s="62"/>
+      <c r="T50" s="123"/>
+      <c r="U50" s="182"/>
+      <c r="V50" s="62"/>
+      <c r="W50" s="202"/>
       <c r="X50" s="3"/>
     </row>
     <row r="51" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
-      <c r="B51" s="63"/>
-      <c r="C51" s="64"/>
-      <c r="D51" s="65"/>
-      <c r="E51" s="88"/>
-      <c r="F51" s="89"/>
-      <c r="G51" s="89"/>
-      <c r="H51" s="90"/>
-      <c r="I51" s="88"/>
-      <c r="J51" s="89"/>
-      <c r="K51" s="90"/>
+      <c r="B51" s="183"/>
+      <c r="C51" s="184"/>
+      <c r="D51" s="185"/>
+      <c r="E51" s="71"/>
+      <c r="F51" s="72"/>
+      <c r="G51" s="72"/>
+      <c r="H51" s="73"/>
+      <c r="I51" s="71"/>
+      <c r="J51" s="72"/>
+      <c r="K51" s="73"/>
       <c r="L51" s="9"/>
       <c r="N51" s="3"/>
-      <c r="O51" s="63"/>
-      <c r="P51" s="64"/>
-      <c r="Q51" s="65"/>
-      <c r="R51" s="63"/>
-      <c r="S51" s="64"/>
-      <c r="T51" s="65"/>
-      <c r="U51" s="63"/>
-      <c r="V51" s="64"/>
-      <c r="W51" s="68"/>
+      <c r="O51" s="183"/>
+      <c r="P51" s="184"/>
+      <c r="Q51" s="185"/>
+      <c r="R51" s="183"/>
+      <c r="S51" s="184"/>
+      <c r="T51" s="185"/>
+      <c r="U51" s="183"/>
+      <c r="V51" s="184"/>
+      <c r="W51" s="203"/>
       <c r="X51" s="3"/>
     </row>
     <row r="52" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
-      <c r="B52" s="178" t="s">
+      <c r="B52" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="178"/>
-      <c r="D52" s="178"/>
-      <c r="E52" s="179" t="s">
+      <c r="C52" s="74"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="F52" s="180"/>
-      <c r="G52" s="180"/>
-      <c r="H52" s="181"/>
-      <c r="I52" s="178" t="s">
+      <c r="F52" s="76"/>
+      <c r="G52" s="76"/>
+      <c r="H52" s="77"/>
+      <c r="I52" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="J52" s="178"/>
-      <c r="K52" s="178"/>
+      <c r="J52" s="74"/>
+      <c r="K52" s="74"/>
       <c r="L52" s="8"/>
       <c r="M52" s="2"/>
       <c r="N52" s="3"/>
-      <c r="O52" s="182" t="s">
+      <c r="O52" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="P52" s="182"/>
-      <c r="Q52" s="182"/>
-      <c r="R52" s="182" t="s">
+      <c r="P52" s="78"/>
+      <c r="Q52" s="78"/>
+      <c r="R52" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="S52" s="182"/>
-      <c r="T52" s="182"/>
-      <c r="U52" s="182" t="s">
+      <c r="S52" s="78"/>
+      <c r="T52" s="78"/>
+      <c r="U52" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="V52" s="182"/>
-      <c r="W52" s="183"/>
+      <c r="V52" s="78"/>
+      <c r="W52" s="79"/>
       <c r="X52" s="3"/>
     </row>
     <row r="53" spans="1:24" ht="43.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6325,61 +6337,85 @@
     </row>
   </sheetData>
   <mergeCells count="167">
-    <mergeCell ref="B29:J30"/>
-    <mergeCell ref="O29:W30"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="R31:W32"/>
-    <mergeCell ref="E48:H51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="E52:H52"/>
-    <mergeCell ref="I52:K52"/>
-    <mergeCell ref="O52:Q52"/>
-    <mergeCell ref="R52:T52"/>
-    <mergeCell ref="U52:W52"/>
-    <mergeCell ref="B31:C32"/>
-    <mergeCell ref="D31:F32"/>
-    <mergeCell ref="G31:J32"/>
-    <mergeCell ref="K31:K32"/>
-    <mergeCell ref="O31:Q32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="F25:K25"/>
-    <mergeCell ref="F26:K26"/>
-    <mergeCell ref="F27:K27"/>
-    <mergeCell ref="O26:Q26"/>
-    <mergeCell ref="O27:Q27"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="O23:Q23"/>
-    <mergeCell ref="O24:Q24"/>
-    <mergeCell ref="O25:Q25"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="F22:K22"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="O37:Q37"/>
+    <mergeCell ref="O38:Q38"/>
+    <mergeCell ref="O39:Q39"/>
+    <mergeCell ref="O40:Q40"/>
+    <mergeCell ref="O41:Q41"/>
+    <mergeCell ref="O42:Q42"/>
+    <mergeCell ref="R48:T51"/>
+    <mergeCell ref="U48:W51"/>
+    <mergeCell ref="P47:W47"/>
+    <mergeCell ref="U26:W26"/>
+    <mergeCell ref="U27:W27"/>
+    <mergeCell ref="B45:K46"/>
+    <mergeCell ref="O45:X46"/>
+    <mergeCell ref="O33:Q33"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="O35:Q35"/>
+    <mergeCell ref="O36:Q36"/>
+    <mergeCell ref="O44:X44"/>
+    <mergeCell ref="O43:Q43"/>
+    <mergeCell ref="R33:W33"/>
+    <mergeCell ref="R34:W34"/>
+    <mergeCell ref="R35:W35"/>
+    <mergeCell ref="R36:W36"/>
+    <mergeCell ref="R37:W37"/>
+    <mergeCell ref="R38:W38"/>
+    <mergeCell ref="R39:W39"/>
+    <mergeCell ref="R40:W40"/>
+    <mergeCell ref="R41:W41"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="R42:W42"/>
+    <mergeCell ref="R43:W43"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="I48:K51"/>
+    <mergeCell ref="B48:D51"/>
+    <mergeCell ref="O48:Q51"/>
+    <mergeCell ref="O28:W28"/>
+    <mergeCell ref="U20:W20"/>
+    <mergeCell ref="U21:W21"/>
+    <mergeCell ref="U22:W22"/>
+    <mergeCell ref="U23:W23"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="U25:W25"/>
+    <mergeCell ref="U5:X5"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="U13:W13"/>
+    <mergeCell ref="U14:W14"/>
+    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="U19:W19"/>
+    <mergeCell ref="U7:X7"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="O14:Q14"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="B8:K8"/>
+    <mergeCell ref="B7:K7"/>
     <mergeCell ref="D38:F38"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="A1:X1"/>
@@ -6404,15 +6440,16 @@
     <mergeCell ref="F15:K15"/>
     <mergeCell ref="F16:K16"/>
     <mergeCell ref="F17:K17"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="O14:Q14"/>
-    <mergeCell ref="O15:Q15"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="F24:K24"/>
+    <mergeCell ref="H4:K4"/>
     <mergeCell ref="R6:T6"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="O21:Q21"/>
@@ -6422,76 +6459,51 @@
     <mergeCell ref="O18:Q18"/>
     <mergeCell ref="O19:Q19"/>
     <mergeCell ref="O20:Q20"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="U5:X5"/>
-    <mergeCell ref="U6:X6"/>
-    <mergeCell ref="U13:W13"/>
-    <mergeCell ref="U14:W14"/>
-    <mergeCell ref="U15:W15"/>
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="U19:W19"/>
-    <mergeCell ref="U7:X7"/>
-    <mergeCell ref="B8:K8"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="I48:K51"/>
-    <mergeCell ref="B48:D51"/>
-    <mergeCell ref="O48:Q51"/>
-    <mergeCell ref="O28:W28"/>
-    <mergeCell ref="U20:W20"/>
-    <mergeCell ref="U21:W21"/>
-    <mergeCell ref="U22:W22"/>
-    <mergeCell ref="U23:W23"/>
-    <mergeCell ref="R21:T21"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="R25:T25"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="U24:W24"/>
-    <mergeCell ref="U25:W25"/>
-    <mergeCell ref="U26:W26"/>
-    <mergeCell ref="U27:W27"/>
-    <mergeCell ref="B45:K46"/>
-    <mergeCell ref="O45:X46"/>
-    <mergeCell ref="O33:Q33"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="O35:Q35"/>
-    <mergeCell ref="O36:Q36"/>
-    <mergeCell ref="O44:X44"/>
-    <mergeCell ref="O43:Q43"/>
-    <mergeCell ref="R33:W33"/>
-    <mergeCell ref="R34:W34"/>
-    <mergeCell ref="R35:W35"/>
-    <mergeCell ref="R36:W36"/>
-    <mergeCell ref="R37:W37"/>
-    <mergeCell ref="R38:W38"/>
-    <mergeCell ref="R39:W39"/>
-    <mergeCell ref="R40:W40"/>
-    <mergeCell ref="R41:W41"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="R42:W42"/>
-    <mergeCell ref="R43:W43"/>
-    <mergeCell ref="O37:Q37"/>
-    <mergeCell ref="O38:Q38"/>
-    <mergeCell ref="O39:Q39"/>
-    <mergeCell ref="O40:Q40"/>
-    <mergeCell ref="O41:Q41"/>
-    <mergeCell ref="O42:Q42"/>
-    <mergeCell ref="R48:T51"/>
-    <mergeCell ref="U48:W51"/>
-    <mergeCell ref="P47:W47"/>
+    <mergeCell ref="F25:K25"/>
+    <mergeCell ref="F26:K26"/>
+    <mergeCell ref="F27:K27"/>
+    <mergeCell ref="O26:Q26"/>
+    <mergeCell ref="O27:Q27"/>
+    <mergeCell ref="R26:T26"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="O23:Q23"/>
+    <mergeCell ref="O24:Q24"/>
+    <mergeCell ref="O25:Q25"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B29:J30"/>
+    <mergeCell ref="O29:W30"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="R31:W32"/>
+    <mergeCell ref="E48:H51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="E52:H52"/>
+    <mergeCell ref="I52:K52"/>
+    <mergeCell ref="O52:Q52"/>
+    <mergeCell ref="R52:T52"/>
+    <mergeCell ref="U52:W52"/>
+    <mergeCell ref="B31:C32"/>
+    <mergeCell ref="D31:F32"/>
+    <mergeCell ref="G31:J32"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="O31:Q32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="E37:F37"/>
   </mergeCells>
   <conditionalFormatting sqref="O21:O26">
     <cfRule type="duplicateValues" dxfId="0" priority="1" stopIfTrue="1"/>
@@ -6503,17 +6515,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dca7b0d4-e4b1-4c05-affe-89d22c055295">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="416ac7e9-f7ad-45a6-b75c-3a7d0b0271c6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008CB83FD72A88CD49BF8A1AFB64ACFF57" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="91fdf7f69dd4288062a5cac7747ce293">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="416ac7e9-f7ad-45a6-b75c-3a7d0b0271c6" xmlns:ns3="dca7b0d4-e4b1-4c05-affe-89d22c055295" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d760217f629fc20119e799cbbc8c74d5" ns2:_="" ns3:_="">
     <xsd:import namespace="416ac7e9-f7ad-45a6-b75c-3a7d0b0271c6"/>
@@ -6748,6 +6749,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dca7b0d4-e4b1-4c05-affe-89d22c055295">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="416ac7e9-f7ad-45a6-b75c-3a7d0b0271c6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6758,17 +6770,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D1DC88E-3653-4319-ABCD-B1AAFFE0078A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dca7b0d4-e4b1-4c05-affe-89d22c055295"/>
-    <ds:schemaRef ds:uri="416ac7e9-f7ad-45a6-b75c-3a7d0b0271c6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2D6178F-E8E5-48CD-ADD8-4A650E976612}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6787,6 +6788,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D1DC88E-3653-4319-ABCD-B1AAFFE0078A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dca7b0d4-e4b1-4c05-affe-89d22c055295"/>
+    <ds:schemaRef ds:uri="416ac7e9-f7ad-45a6-b75c-3a7d0b0271c6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AAD2324-1C6D-4A91-8CD0-9F8D64F04198}">
   <ds:schemaRefs>

</xml_diff>